<commit_message>
updated source files and added propellant properties.xlsx
</commit_message>
<xml_diff>
--- a/Avionics/EngineControlUnit/PCB/Converse ECU controller requirements.xlsx
+++ b/Avionics/EngineControlUnit/PCB/Converse ECU controller requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/EngineControlUnit/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62FA1F5D-91D4-D144-BFFE-5C3734D2C5EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC43C4CB-A441-6247-A6E9-8D29395F943A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{C4B5CCE9-66F1-694B-8BDE-ED37BD957B63}"/>
   </bookViews>
@@ -24,11 +24,76 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+  <si>
+    <t>ECU CONTROLLER REQUIREMENTS</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Component </t>
+  </si>
+  <si>
+    <t>Channel Requirement</t>
+  </si>
+  <si>
+    <t>External Storage</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Type/Purpose</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Lithium ion Battery</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Spark igniter</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -55,8 +120,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +443,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45971728-C6E2-044B-886B-FC679701BD42}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>